<commit_message>
Categories and about us added
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>صفحه سرچ</t>
   </si>
@@ -42,12 +42,6 @@
   </si>
   <si>
     <t>صفحه نمایش محصول</t>
-  </si>
-  <si>
-    <t>صفحه ارتباط با ما</t>
-  </si>
-  <si>
-    <t>صفحه تماس با ما</t>
   </si>
   <si>
     <t>صفحه درباره ما</t>
@@ -380,7 +374,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,6 +396,9 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -421,24 +418,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit user info , userpanel , card pages done
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>صفحه سرچ</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>صفحه دسته بندی ها</t>
+  </si>
+  <si>
+    <t>صفحه سبد خرید</t>
+  </si>
+  <si>
+    <t>صغحه ویرایش اطلاعات کاربر</t>
   </si>
 </sst>
 </file>
@@ -374,7 +380,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,6 +415,9 @@
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -418,6 +427,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+    </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
@@ -429,6 +454,9 @@
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
header changed adminpanel and login done
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>صفحه سرچ</t>
   </si>
@@ -54,6 +54,36 @@
   </si>
   <si>
     <t>صغحه ویرایش اطلاعات کاربر</t>
+  </si>
+  <si>
+    <t>تنظیمات تبلیغات</t>
+  </si>
+  <si>
+    <t>تنظیم 3 پست بزرگ صفحه اصلی</t>
+  </si>
+  <si>
+    <t>تنظیمات اسلایدر پایین صفحه</t>
+  </si>
+  <si>
+    <t>افزودن کالا</t>
+  </si>
+  <si>
+    <t>تنظیمات دسته بندی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ادیت اطلاعات فروشگاه و توضیحات </t>
+  </si>
+  <si>
+    <t>تغییر اطلاعات برای مدیر سایت</t>
+  </si>
+  <si>
+    <t>صفحه ورود</t>
+  </si>
+  <si>
+    <t>ثبت نام</t>
+  </si>
+  <si>
+    <t>صفحه فراموشی کلمه عبور</t>
   </si>
 </sst>
 </file>
@@ -377,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,6 +440,9 @@
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -457,6 +490,59 @@
       </c>
       <c r="B9" s="2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>